<commit_message>
update status in classroom
</commit_message>
<xml_diff>
--- a/Quy dinh.xlsx
+++ b/Quy dinh.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="122211" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>int</t>
   </si>
@@ -73,6 +73,18 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>classroom</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>close</t>
   </si>
 </sst>
 </file>
@@ -149,33 +161,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:E12"/>
+  <dimension ref="A3:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,144 +504,170 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="8"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="4" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>1</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="2">
         <v>1</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="7">
+      <c r="A6" s="4"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="2">
         <v>2</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="7">
+      <c r="A7" s="4"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="2">
         <v>3</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+      <c r="A8" s="6">
         <v>2</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="2">
         <v>1</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="7">
+      <c r="A9" s="7"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="2">
         <v>2</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="A10" s="4">
         <v>3</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="2">
         <v>0</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="7">
+      <c r="A11" s="4"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="2">
         <v>1</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="7">
+      <c r="A12" s="4"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="2">
         <v>2</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="2" t="s">
         <v>17</v>
       </c>
     </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>4</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="10">
+        <v>0</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="10">
+        <v>1</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="A10:A12"/>
+  <mergeCells count="16">
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="D3:E3"/>
@@ -637,8 +676,14 @@
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A10:A12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>